<commit_message>
modified the FA table
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/210824_FAMES_pot_LW_publication.xlsx
+++ b/analysis/data/raw_data/210824_FAMES_pot_LW_publication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/GJBpottery/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0901A771-4E0B-FF4A-99EF-92F0D94137C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD9B3BE-C9A7-694B-94F5-4A134A732654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29180" yWindow="4340" windowWidth="33700" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37480" yWindow="720" windowWidth="24000" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>lyw Pottery FAME II</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>ng C18:1</t>
+  </si>
+  <si>
+    <t>g extracted</t>
   </si>
 </sst>
 </file>
@@ -551,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E051E140-E4E6-EA4A-B35E-019129C46E0F}">
-  <dimension ref="A1:AP19"/>
+  <dimension ref="A1:AQ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="AP4" sqref="AP4"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="AP9" sqref="AP9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -568,7 +571,7 @@
     <col min="41" max="41" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +581,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>21.6</v>
       </c>
@@ -637,7 +640,7 @@
         <v>51.2</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>17</v>
       </c>
@@ -758,8 +761,11 @@
       <c r="AP3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -862,11 +868,14 @@
         <v>0.31675875791749675</v>
       </c>
       <c r="AP4">
-        <f xml:space="preserve"> (W4+X4+Y4+AA4+AB4+AE4+AD4+AG4+AC4+AH4+AI4+AJ4+AK4+AL4+Z4)/1000</f>
-        <v>19.426299847889617</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> SUM(W4:AL4)/AO4/AQ4/1000</f>
+        <v>17.373477299361944</v>
+      </c>
+      <c r="AQ4">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -954,11 +963,14 @@
         <v>0.23297951998893873</v>
       </c>
       <c r="AP5">
-        <f xml:space="preserve"> (W5+X5+Y5+AA5+AB5+AE5+AD5+AG5+AC5+AH5+AI5+AJ5+AK5+AL5+Z5)/1000</f>
-        <v>7.2631386971659619</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AP5:AP9" si="10" xml:space="preserve"> SUM(W5:AL5)/AO5/AQ5/1000</f>
+        <v>8.8565367266152997</v>
+      </c>
+      <c r="AQ5">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1040,11 +1052,14 @@
         <v>0.21228069836392888</v>
       </c>
       <c r="AP6">
-        <f xml:space="preserve"> (W6+X6+Y6+AA6+AB6+AE6+AD6+AG6+AC6+AH6+AI6+AJ6+AK6+AL6+Z6)/1000</f>
-        <v>5.1756326505809671</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+        <f t="shared" si="10"/>
+        <v>6.9859827558054048</v>
+      </c>
+      <c r="AQ6">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1133,11 +1148,14 @@
         <v>0.13779981801267924</v>
       </c>
       <c r="AP7">
-        <f xml:space="preserve"> (W7+X7+Y7+AA7+AB7+AM7+AE7+AD7+AG7+AC7+AH7+AI7+AJ7+AK7+AL7+Z7)/1000</f>
-        <v>7.1923913481364954</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+        <f t="shared" si="10"/>
+        <v>12.242869314535945</v>
+      </c>
+      <c r="AQ7">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1210,7 +1228,7 @@
         <v>1242.6087819308641</v>
       </c>
       <c r="X8" s="3">
-        <f t="shared" ref="X8" si="10" xml:space="preserve"> D8*V8*100/5</f>
+        <f t="shared" ref="X8" si="11" xml:space="preserve"> D8*V8*100/5</f>
         <v>451.45191266261946</v>
       </c>
       <c r="Y8" s="3">
@@ -1234,7 +1252,7 @@
         <v>9554.4789715087099</v>
       </c>
       <c r="AD8" s="3">
-        <f t="shared" ref="AD8:AD9" si="11">J8*V8*100/5</f>
+        <f t="shared" ref="AD8:AD9" si="12">J8*V8*100/5</f>
         <v>4659.3040057564558</v>
       </c>
       <c r="AE8" s="3">
@@ -1282,11 +1300,14 @@
         <v>0.87971395315291867</v>
       </c>
       <c r="AP8">
-        <f xml:space="preserve"> (W8+X8+Y8+AA8+AB8+AE8+AD8+AG8+AC8+AH8+AI8+AJ8+AK8+AL8+Z8+AF8)/1000</f>
-        <v>152.7681530563664</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+        <f t="shared" si="10"/>
+        <v>48.643311365368774</v>
+      </c>
+      <c r="AQ8">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1350,7 +1371,7 @@
       </c>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>84.725724833238559</v>
       </c>
       <c r="AE9" s="3">
@@ -1380,11 +1401,14 @@
         <v>6.5546228289963995E-2</v>
       </c>
       <c r="AP9">
-        <f xml:space="preserve"> (W9+X9+Y9+AA9+AB9+AE9+AD9+AG9+AC9+AH9+AI9+AJ9+AK9+AL9+Z9)/1000</f>
-        <v>4.3352851672013335</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+        <f t="shared" si="10"/>
+        <v>18.790022499389757</v>
+      </c>
+      <c r="AQ9">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1439,23 +1463,23 @@
       <c r="AN10" s="3"/>
       <c r="AO10" s="2"/>
       <c r="AP10">
-        <f t="shared" ref="AP10" si="12" xml:space="preserve"> (W10+X10+Y10+AA10+AB10+AM10+AE10+AD10+AG10+AC10+AH10+AI10+AJ10+AK10+AL10+Z10)/1000</f>
-        <v>3.7584546282883977</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AP5:AP10" si="13" xml:space="preserve"> SUM(W10:AL10)/1000</f>
+        <v>2.4495612773905844</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="12:12" x14ac:dyDescent="0.2">

</xml_diff>